<commit_message>
sunday 23 march push to branch darshana
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Excel_Login_Pythoncode.xlsx
+++ b/src/test/resources/TestData/Excel_Login_Pythoncode.xlsx
@@ -196,10 +196,10 @@
     <t xml:space="preserve">jvjd</t>
   </si>
   <si>
-    <t xml:space="preserve">dashanaBhen</t>
+    <t xml:space="preserve">meenakanan</t>
   </si>
   <si>
-    <t xml:space="preserve">sdet2batch</t>
+    <t xml:space="preserve">sdet199batch</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
monday commit to branch darshana
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Excel_Login_Pythoncode.xlsx
+++ b/src/test/resources/TestData/Excel_Login_Pythoncode.xlsx
@@ -196,10 +196,10 @@
     <t xml:space="preserve">jvjd</t>
   </si>
   <si>
-    <t xml:space="preserve">meenakanan</t>
+    <t xml:space="preserve">irabhende</t>
   </si>
   <si>
-    <t xml:space="preserve">sdet199batch</t>
+    <t xml:space="preserve">sdet19batch</t>
   </si>
 </sst>
 </file>

</xml_diff>